<commit_message>
finalização do projeto: criação do banco de dados, criação dos gráficos e pipelines
</commit_message>
<xml_diff>
--- a/produtos_scrape.xlsx
+++ b/produtos_scrape.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,11 +514,6 @@
           <t>preco_debug</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>preco_fontes</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -549,26 +544,18 @@
           <t>KaBuM!</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3,3 de 5</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:01</t>
+          <t>2025-11-01 21:34:27</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>9.5</v>
+        <v>5.23</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -578,12 +565,7 @@
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>R$ 3.099,00 | 3099.0 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 1,88 | 1.88 | score=3 | context:por/avista; R$ 3,35 | 3.35 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 3.099,00 | 3099.0 | jsonld</t>
         </is>
       </c>
     </row>
@@ -624,20 +606,16 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:11</t>
+          <t>2025-11-01 21:34:31</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>7.99</v>
+        <v>3.04</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -647,12 +625,7 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>R$ 9.899,10 | 9899.1 | score=5 | jsonld; R$ 0,10 | 0.1 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 9.899,10 | 9899.1 | jsonld</t>
         </is>
       </c>
     </row>
@@ -680,29 +653,25 @@
       <c r="E4" t="n">
         <v>4799</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Magalu</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>4,86 de 5</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1356</v>
+        <v>1367</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:14</t>
+          <t>2025-11-01 21:34:35</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2.28</v>
+        <v>2.61</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -712,12 +681,7 @@
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>R$ 4.799,00 | 4799.0 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.799,00 | 4799.0 | jsonld; R$ 5.332,22 | 5332.22 | sel:[data-testid*="price"]; R$ 9.999,00 | 9999.0 | sel:[data-testid*="price"]; R$ 9.999,00 | 9999.0 | sel:[data-testid*="price"]; R$ 9.999,00 | 9999.0 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -752,20 +716,16 @@
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:23</t>
+          <t>2025-11-01 21:34:41</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>7.22</v>
+        <v>5.38</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -775,12 +735,7 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>R$ 3.199,99 | 3199.99 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 3.199,99 | 3199.99 | jsonld</t>
         </is>
       </c>
     </row>
@@ -802,35 +757,29 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 43,51</t>
+          <t>R$ 1.509,00</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>43.51</v>
+        <v>1509</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>31</v>
-      </c>
+          <t>loja parceira e entregue pelo Magalu</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:28</t>
+          <t>2025-11-01 21:34:44</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>3.2</v>
+        <v>2.24</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -840,12 +789,7 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 1.509,00 | 1509.0 | sel:[data-testid*="price"]; R$ 1.739,00 | 1739.0 | sel:[data-testid*="price"]; R$ 1.739,00 | 1739.0 | sel:[data-testid*="price"]; R$ 1.739,00 | 1739.0 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -886,20 +830,16 @@
       <c r="H7" t="n">
         <v>30</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:37</t>
+          <t>2025-11-01 21:34:50</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>8.58</v>
+        <v>5.59</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -909,12 +849,7 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>R$ 2.370,57 | 2370.57 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,53 | 0.53 | score=3 | context:por/avista; R$ 17,78 | 17.78 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.370,57 | 2370.57 | jsonld</t>
         </is>
       </c>
     </row>
@@ -936,15 +871,15 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 2.422,50</t>
+          <t>R$ 260,00</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2422.5</v>
+        <v>260</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Magalu</t>
+          <t>loja parceira e entregue pelo Magalu</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -960,11 +895,11 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:42</t>
+          <t>2025-11-01 21:34:53</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>3.06</v>
+        <v>1.81</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -974,12 +909,7 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>R$ 2.422,50 | 2422.5 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 260,00 | 260.0 | sel:[data-testid*="price"]; R$ 2.339,99 | 2339.99 | sel:[data-testid*="price"]; R$ 2.339,99 | 2339.99 | sel:[data-testid*="price"]; R$ 2.371,50 | 2371.5 | jsonld; R$ 2.550,00 | 2550.0 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1012,22 +942,18 @@
           <t>KaBuM!</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>123,7 de 5</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:49</t>
+          <t>2025-11-01 21:35:03</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>6.48</v>
+        <v>9.23</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1037,12 +963,7 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>R$ 4.403,79 | 4403.79 | score=5 | jsonld; R$ 0,42 | 0.42 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.403,79 | 4403.79 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1075,22 +996,18 @@
           <t>KaBuM!</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5,1 de 5</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:55</t>
+          <t>2025-11-01 21:35:07</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>4.19</v>
+        <v>2.59</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1100,12 +1017,7 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>R$ 3.935,04 | 3935.04 | score=5 | jsonld; R$ 0,10 | 0.1 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,50 | 0.5 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 3.935,04 | 3935.04 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1127,17 +1039,13 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 4.769,10</t>
+          <t>R$ 4.679,10</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4769.1</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Magalu</t>
-        </is>
-      </c>
+        <v>4679.1</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>5</t>
@@ -1151,11 +1059,11 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-10-30 11:41:59</t>
+          <t>2025-11-01 21:35:09</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>3.25</v>
+        <v>1.83</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1165,12 +1073,7 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>R$ 4.769,10 | 4769.1 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.679,10 | 4679.1 | jsonld; R$ 5.199,00 | 5199.0 | sel:[data-testid*="price"]; R$ 7.080,00 | 7080.0 | sel:[data-testid*="price"]; R$ 7.080,00 | 7080.0 | sel:[data-testid*="price"]; R$ 7.080,00 | 7080.0 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1205,20 +1108,16 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:09</t>
+          <t>2025-11-01 21:35:13</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>8.17</v>
+        <v>2.8</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1228,12 +1127,7 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>R$ 4.799,00 | 4799.0 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.799,00 | 4799.0 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1253,37 +1147,25 @@
           <t>LINK MAGALU</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>R$ 43,51</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>43.51</v>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>21</v>
-      </c>
+          <t>loja parceira</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:13</t>
+          <t>2025-11-01 21:35:16</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>2.95</v>
+        <v>2.36</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1291,16 +1173,7 @@
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
-        </is>
-      </c>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1344,11 +1217,11 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:19</t>
+          <t>2025-11-01 21:35:21</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>5.15</v>
+        <v>3.96</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1358,12 +1231,7 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>R$ 4.099,90 | 4099.9 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,50 | 0.5 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.099,90 | 4099.9 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1385,35 +1253,31 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 3.533,91</t>
+          <t>R$ 3.579,57</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3533.91</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Magalu</t>
-        </is>
-      </c>
+        <v>3579.57</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>4,68 de 5</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:24</t>
+          <t>2025-11-01 21:35:24</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>3.25</v>
+        <v>2.05</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1423,12 +1287,7 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>R$ 3.533,91 | 3533.91 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 3.579,57 | 3579.57 | jsonld; R$ 3.849,00 | 3849.0 | sel:[data-testid*="price"]; R$ 3.999,90 | 3999.9 | sel:[data-testid*="price"]; R$ 3.999,90 | 3999.9 | sel:[data-testid*="price"]; R$ 3.999,90 | 3999.9 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1463,20 +1322,16 @@
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:32</t>
+          <t>2025-11-01 21:35:29</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>7.75</v>
+        <v>4.04</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1486,12 +1341,7 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>R$ 2.519,10 | 2519.1 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.519,10 | 2519.1 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1513,33 +1363,29 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R$ 43,51</t>
+          <t>R$ 2.754,15</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>43.51</v>
+        <v>2754.15</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>999,00 de 5</t>
-        </is>
-      </c>
+          <t>loja parceira e entregue pelo Magalu</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:36</t>
+          <t>2025-11-01 21:35:32</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>3.06</v>
+        <v>1.84</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1549,12 +1395,7 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.754,15 | 2754.15 | sel:[data-testid*="price"]; R$ 2.999,00 | 2999.0 | sel:[data-testid*="price"]; R$ 2.999,00 | 2999.0 | sel:[data-testid*="price"]; R$ 2.999,00 | 2999.0 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1595,20 +1436,16 @@
       <c r="H18" t="n">
         <v>49</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:45</t>
+          <t>2025-11-01 21:35:36</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>7.58</v>
+        <v>3.15</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -1618,12 +1455,7 @@
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>R$ 4.184,07 | 4184.07 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 4.184,07 | 4184.07 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1664,20 +1496,16 @@
       <c r="H19" t="n">
         <v>1</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:54</t>
+          <t>2025-11-01 21:35:40</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>7.2</v>
+        <v>3.08</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1687,12 +1515,7 @@
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>R$ 2.449,00 | 2449.0 | score=5 | jsonld; R$ 0,10 | 0.1 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.449,00 | 2449.0 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1714,35 +1537,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R$ 29,90</t>
+          <t>R$ 248,90</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>29.9</v>
+        <v>248.9</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>56</v>
-      </c>
+          <t>loja parceira e entregue pelo Magalu</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2025-10-30 11:42:58</t>
+          <t>2025-11-01 21:35:43</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>3.3</v>
+        <v>1.93</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -1752,12 +1569,7 @@
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>R$ 29,90 | 29.9 | score=3 | context:por/avista; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista; R$ 136,40 | 136.4 | score=0 | sel:[data-testid*="price"]</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 248,90 | 248.9 | sel:[data-testid*="price"]; R$ 2.240,10 | 2240.1 | sel:[data-testid*="price"]; R$ 2.240,10 | 2240.1 | sel:[data-testid*="price"]; R$ 2.857,17 | 2857.17 | sel:[data-testid*="price"]; R$ 3.498,83 | 3498.83 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1779,11 +1591,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>R$ 2.299,00</t>
+          <t>R$ 2.289,99</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2299</v>
+        <v>2289.99</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1798,20 +1610,16 @@
       <c r="H21" t="n">
         <v>65</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:07</t>
+          <t>2025-11-01 21:35:47</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>7.53</v>
+        <v>3.26</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -1821,12 +1629,7 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>R$ 2.299,00 | 2299.0 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.289,99 | 2289.99 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1848,15 +1651,15 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R$ 2.299,00</t>
+          <t>R$ 131,17</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2299</v>
+        <v>131.17</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Magalu</t>
+          <t>loja parceira e entregue pelo Magalu</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1865,18 +1668,18 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:11</t>
+          <t>2025-11-01 21:35:49</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>3.04</v>
+        <v>2.11</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -1886,12 +1689,7 @@
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>R$ 2.299,00 | 2299.0 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 131,17 | 131.17 | sel:[data-testid*="price"]; R$ 131,17 | 131.17 | sel:[data-testid*="price"]; R$ 224,90 | 224.9 | sel:[data-testid*="price"]; R$ 393,51 | 393.51 | sel:[data-testid*="price"]; R$ 393,51 | 393.51 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -1913,11 +1711,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R$ 1.899,99</t>
+          <t>R$ 2.099,00</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1899.99</v>
+        <v>2099</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1932,20 +1730,16 @@
       <c r="H23" t="n">
         <v>18</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:19</t>
+          <t>2025-11-01 21:35:54</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>7.46</v>
+        <v>3.53</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -1955,12 +1749,7 @@
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>R$ 1.899,99 | 1899.99 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,54 | 0.54 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.099,00 | 2099.0 | jsonld</t>
         </is>
       </c>
     </row>
@@ -1982,35 +1771,31 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>R$ 2.374,05</t>
+          <t>R$ 131,17</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2374.05</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Magalu</t>
-        </is>
-      </c>
+        <v>131.17</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>4,92 de 5</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:23</t>
+          <t>2025-11-01 21:35:56</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>2.83</v>
+        <v>1.97</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -2020,12 +1805,7 @@
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>R$ 2.374,05 | 2374.05 | score=5 | jsonld; R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista; R$ 5,25 | 5.25 | score=1 | context:por/avista; R$ 5,25 | 5.25 | score=1 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 131,17 | 131.17 | sel:[data-testid*="price"]; R$ 131,17 | 131.17 | sel:[data-testid*="price"]; R$ 185,03 | 185.03 | sel:[data-testid*="price"]; R$ 393,51 | 393.51 | sel:[data-testid*="price"]; R$ 393,51 | 393.51 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -2071,11 +1851,11 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:28</t>
+          <t>2025-11-01 21:36:00</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>3.74</v>
+        <v>3.14</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -2085,12 +1865,7 @@
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>R$ 2.698,20 | 2698.2 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,50 | 0.5 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.698,20 | 2698.2 | jsonld</t>
         </is>
       </c>
     </row>
@@ -2110,37 +1885,25 @@
           <t>LINK MAGALU</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>R$ 43,51</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>43.51</v>
-      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>5</v>
-      </c>
+          <t>loja parceira</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:32</t>
+          <t>2025-11-01 21:36:03</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>2.97</v>
+        <v>1.78</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -2148,16 +1911,7 @@
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista; R$ 18,47 | 18.47 | score=2 | sel:[data-testid*="price"]; R$ 38,90 | 38.9 | score=2 | sel:[data-testid*="price"]; R$ 39,81 | 39.81 | score=2 | sel:[data-testid*="price"]</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
-        </is>
-      </c>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2177,11 +1931,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R$ 2.789,10</t>
+          <t>R$ 2.429,10</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2789.1</v>
+        <v>2429.1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2196,20 +1950,16 @@
       <c r="H27" t="n">
         <v>1</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:42</t>
+          <t>2025-11-01 21:36:06</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>8.35</v>
+        <v>2.7</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -2219,12 +1969,7 @@
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>R$ 2.789,10 | 2789.1 | score=5 | jsonld; R$ 0,11 | 0.11 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,53 | 0.53 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 2.429,10 | 2429.1 | jsonld</t>
         </is>
       </c>
     </row>
@@ -2246,11 +1991,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R$ 929,99</t>
+          <t>R$ 1.389,83</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>929.99</v>
+        <v>1389.83</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2265,20 +2010,16 @@
       <c r="H28" t="n">
         <v>789</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:53</t>
+          <t>2025-11-01 21:36:11</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>9.890000000000001</v>
+        <v>3.06</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2288,12 +2029,7 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t>R$ 929,99 | 929.99 | score=5 | jsonld; R$ 0,10 | 0.1 | score=3 | context:por/avista; R$ 0,20 | 0.2 | score=3 | context:por/avista; R$ 0,52 | 0.52 | score=3 | context:por/avista; R$ 44,44 | 44.44 | score=3 | context:por/avista; R$ 255,25 | 255.25 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 1.389,83 | 1389.83 | jsonld</t>
         </is>
       </c>
     </row>
@@ -2315,35 +2051,29 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>R$ 43,51</t>
+          <t>R$ 1.544,26</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>43.51</v>
+        <v>1544.26</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>169</v>
-      </c>
+          <t>loja parceira e entregue pelo Magalu</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2025-10-30 11:43:58</t>
+          <t>2025-11-01 21:36:13</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>3.6</v>
+        <v>1.66</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
@@ -2353,12 +2083,7 @@
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista; R$ 15.244.117,20 | 15244117.2 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 1.544,26 | 1544.26 | sel:[data-testid*="price"]; R$ 1.544,26 | 1544.26 | sel:[data-testid*="price"]; R$ 1.544,26 | 1544.26 | sel:[data-testid*="price"]; R$ 1.544,26 | 1544.26 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>
@@ -2380,33 +2105,29 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>R$ 43,51</t>
+          <t>R$ 9.998,95</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>43.51</v>
+        <v>9998.950000000001</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Magalu</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>104,21 de 5</t>
-        </is>
-      </c>
+          <t>loja parceira e entregue pelo Magalu</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2025-10-30 11:44:02</t>
+          <t>2025-11-01 21:36:16</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>3.16</v>
+        <v>1.69</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -2416,12 +2137,7 @@
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>R$ 43,51 | 43.51 | score=3 | context:por/avista; R$ 59,13 | 59.13 | score=3 | context:por/avista</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>jsonld&gt;dom&gt;regex</t>
+          <t>R$ 9.998,95 | 9998.95 | sel:[data-testid*="price"]; R$ 10.104,21 | 10104.21 | sel:[data-testid*="price"]; R$ 10.104,21 | 10104.21 | sel:[data-testid*="price"]; R$ 10.104,21 | 10104.21 | sel:[data-testid*="price"]</t>
         </is>
       </c>
     </row>

</xml_diff>